<commit_message>
Change to single region to match DD files
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\times-ireland-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\times-ireland-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3AC475-EA9C-4B78-BB64-321C448CD709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F208A0A1-9534-4798-A8D6-053FF73568D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -1191,7 +1191,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4251,7 +4251,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -7102,7 +7102,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -7144,116 +7144,116 @@
       </c>
       <c r="D3" s="2" t="str">
         <f t="array" ref="D3">IF(INDEX(D5:D7,$A$4)&lt;&gt;0,INDEX(D5:D7,$A$4),"")</f>
-        <v>National</v>
+        <v/>
       </c>
       <c r="E3" s="2" t="str">
         <f t="array" ref="E3">IF(INDEX(E5:E7,$A$4)&lt;&gt;0,INDEX(E5:E7,$A$4),"")</f>
-        <v>IE-CW</v>
+        <v/>
       </c>
       <c r="F3" s="2" t="str">
         <f t="array" ref="F3">IF(INDEX(F5:F7,$A$4)&lt;&gt;0,INDEX(F5:F7,$A$4),"")</f>
-        <v>IE-D</v>
+        <v/>
       </c>
       <c r="G3" s="2" t="str">
         <f t="array" ref="G3">IF(INDEX(G5:G7,$A$4)&lt;&gt;0,INDEX(G5:G7,$A$4),"")</f>
-        <v>IE-KE</v>
+        <v/>
       </c>
       <c r="H3" s="2" t="str">
         <f t="array" ref="H3">IF(INDEX(H5:H7,$A$4)&lt;&gt;0,INDEX(H5:H7,$A$4),"")</f>
-        <v>IE-KK</v>
+        <v/>
       </c>
       <c r="I3" s="2" t="str">
         <f t="array" ref="I3">IF(INDEX(I5:I7,$A$4)&lt;&gt;0,INDEX(I5:I7,$A$4),"")</f>
-        <v>IE-LS</v>
+        <v/>
       </c>
       <c r="J3" s="2" t="str">
         <f t="array" ref="J3">IF(INDEX(J5:J7,$A$4)&lt;&gt;0,INDEX(J5:J7,$A$4),"")</f>
-        <v>IE-LD</v>
+        <v/>
       </c>
       <c r="K3" s="2" t="str">
         <f t="array" ref="K3">IF(INDEX(K5:K7,$A$4)&lt;&gt;0,INDEX(K5:K7,$A$4),"")</f>
-        <v>IE-LH</v>
+        <v/>
       </c>
       <c r="L3" s="2" t="str">
         <f t="array" ref="L3">IF(INDEX(L5:L7,$A$4)&lt;&gt;0,INDEX(L5:L7,$A$4),"")</f>
-        <v>IE-MH</v>
+        <v/>
       </c>
       <c r="M3" s="2" t="str">
         <f t="array" ref="M3">IF(INDEX(M5:M7,$A$4)&lt;&gt;0,INDEX(M5:M7,$A$4),"")</f>
-        <v>IE-OY</v>
+        <v/>
       </c>
       <c r="N3" s="2" t="str">
         <f t="array" ref="N3">IF(INDEX(N5:N7,$A$4)&lt;&gt;0,INDEX(N5:N7,$A$4),"")</f>
-        <v>IE-WH</v>
+        <v/>
       </c>
       <c r="O3" s="2" t="str">
         <f t="array" ref="O3">IF(INDEX(O5:O7,$A$4)&lt;&gt;0,INDEX(O5:O7,$A$4),"")</f>
-        <v>IE-WX</v>
+        <v/>
       </c>
       <c r="P3" s="2" t="str">
         <f t="array" ref="P3">IF(INDEX(P5:P7,$A$4)&lt;&gt;0,INDEX(P5:P7,$A$4),"")</f>
-        <v>IE-WW</v>
+        <v/>
       </c>
       <c r="Q3" s="2" t="str">
         <f t="array" ref="Q3">IF(INDEX(Q5:Q7,$A$4)&lt;&gt;0,INDEX(Q5:Q7,$A$4),"")</f>
-        <v>IE-CE</v>
+        <v/>
       </c>
       <c r="R3" s="2" t="str">
         <f t="array" ref="R3">IF(INDEX(R5:R7,$A$4)&lt;&gt;0,INDEX(R5:R7,$A$4),"")</f>
-        <v>IE-CO</v>
+        <v/>
       </c>
       <c r="S3" s="2" t="str">
         <f t="array" ref="S3">IF(INDEX(S5:S7,$A$4)&lt;&gt;0,INDEX(S5:S7,$A$4),"")</f>
-        <v>IE-KY</v>
+        <v/>
       </c>
       <c r="T3" s="2" t="str">
         <f t="array" ref="T3">IF(INDEX(T5:T7,$A$4)&lt;&gt;0,INDEX(T5:T7,$A$4),"")</f>
-        <v>IE-LK</v>
+        <v/>
       </c>
       <c r="U3" s="2" t="str">
         <f t="array" ref="U3">IF(INDEX(U5:U7,$A$4)&lt;&gt;0,INDEX(U5:U7,$A$4),"")</f>
-        <v>IE-TA</v>
+        <v/>
       </c>
       <c r="V3" s="2" t="str">
         <f t="array" ref="V3">IF(INDEX(V5:V7,$A$4)&lt;&gt;0,INDEX(V5:V7,$A$4),"")</f>
-        <v>IE-WD</v>
+        <v/>
       </c>
       <c r="W3" s="2" t="str">
         <f t="array" ref="W3">IF(INDEX(W5:W7,$A$4)&lt;&gt;0,INDEX(W5:W7,$A$4),"")</f>
-        <v>IE-G</v>
+        <v/>
       </c>
       <c r="X3" s="2" t="str">
         <f t="array" ref="X3">IF(INDEX(X5:X7,$A$4)&lt;&gt;0,INDEX(X5:X7,$A$4),"")</f>
-        <v>IE-LM</v>
+        <v/>
       </c>
       <c r="Y3" s="2" t="str">
         <f t="array" ref="Y3">IF(INDEX(Y5:Y7,$A$4)&lt;&gt;0,INDEX(Y5:Y7,$A$4),"")</f>
-        <v>IE-MO</v>
+        <v/>
       </c>
       <c r="Z3" s="2" t="str">
         <f t="array" ref="Z3">IF(INDEX(Z5:Z7,$A$4)&lt;&gt;0,INDEX(Z5:Z7,$A$4),"")</f>
-        <v>IE-RN</v>
+        <v/>
       </c>
       <c r="AA3" s="2" t="str">
         <f t="array" ref="AA3">IF(INDEX(AA5:AA7,$A$4)&lt;&gt;0,INDEX(AA5:AA7,$A$4),"")</f>
-        <v>IE-SO</v>
+        <v/>
       </c>
       <c r="AB3" s="2" t="str">
         <f t="array" ref="AB3">IF(INDEX(AB5:AB7,$A$4)&lt;&gt;0,INDEX(AB5:AB7,$A$4),"")</f>
-        <v>IE-CN</v>
+        <v/>
       </c>
       <c r="AC3" s="2" t="str">
         <f t="array" ref="AC3">IF(INDEX(AC5:AC7,$A$4)&lt;&gt;0,INDEX(AC5:AC7,$A$4),"")</f>
-        <v>IE-DL</v>
+        <v/>
       </c>
       <c r="AD3" s="2" t="str">
         <f t="array" ref="AD3">IF(INDEX(AD5:AD7,$A$4)&lt;&gt;0,INDEX(AD5:AD7,$A$4),"")</f>
-        <v>IE-MN</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1"/>
     </row>
@@ -7886,7 +7886,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="str">
         <f>Regions!D3</f>
-        <v>National</v>
+        <v/>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -7915,7 +7915,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="str">
         <f>Regions!E3</f>
-        <v>IE-CW</v>
+        <v/>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -7944,7 +7944,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="str">
         <f>Regions!F3</f>
-        <v>IE-D</v>
+        <v/>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -7973,7 +7973,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="str">
         <f>Regions!G3</f>
-        <v>IE-KE</v>
+        <v/>
       </c>
       <c r="K9">
         <v>4</v>
@@ -7999,7 +7999,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="str">
         <f>Regions!H3</f>
-        <v>IE-KK</v>
+        <v/>
       </c>
       <c r="K10">
         <v>5</v>
@@ -8025,7 +8025,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="str">
         <f>Regions!I3</f>
-        <v>IE-LS</v>
+        <v/>
       </c>
       <c r="E11" s="7"/>
       <c r="K11">
@@ -8052,7 +8052,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="str">
         <f>Regions!J3</f>
-        <v>IE-LD</v>
+        <v/>
       </c>
       <c r="E12" s="7"/>
       <c r="K12">
@@ -8073,7 +8073,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="str">
         <f>Regions!K3</f>
-        <v>IE-LH</v>
+        <v/>
       </c>
       <c r="E13" s="7"/>
       <c r="K13">
@@ -8094,7 +8094,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="str">
         <f>Regions!L3</f>
-        <v>IE-MH</v>
+        <v/>
       </c>
       <c r="E14" s="7"/>
       <c r="K14">
@@ -8115,7 +8115,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="str">
         <f>Regions!M3</f>
-        <v>IE-OY</v>
+        <v/>
       </c>
       <c r="E15" s="7"/>
       <c r="K15">
@@ -8136,7 +8136,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="str">
         <f>Regions!N3</f>
-        <v>IE-WH</v>
+        <v/>
       </c>
       <c r="E16" s="7"/>
       <c r="K16">
@@ -8157,7 +8157,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="str">
         <f>Regions!O3</f>
-        <v>IE-WX</v>
+        <v/>
       </c>
       <c r="E17" s="7"/>
       <c r="Q17">
@@ -8172,7 +8172,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="str">
         <f>Regions!P3</f>
-        <v>IE-WW</v>
+        <v/>
       </c>
       <c r="Q18">
         <v>13</v>
@@ -8186,7 +8186,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="str">
         <f>Regions!Q3</f>
-        <v>IE-CE</v>
+        <v/>
       </c>
       <c r="Q19">
         <v>14</v>
@@ -8199,7 +8199,7 @@
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="str">
         <f>Regions!R3</f>
-        <v>IE-CO</v>
+        <v/>
       </c>
       <c r="Q20">
         <v>15</v>
@@ -8212,7 +8212,7 @@
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="str">
         <f>Regions!S3</f>
-        <v>IE-KY</v>
+        <v/>
       </c>
       <c r="Q21">
         <v>16</v>
@@ -8225,7 +8225,7 @@
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="str">
         <f>Regions!T3</f>
-        <v>IE-LK</v>
+        <v/>
       </c>
       <c r="Q22">
         <v>17</v>
@@ -8238,7 +8238,7 @@
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="str">
         <f>Regions!U3</f>
-        <v>IE-TA</v>
+        <v/>
       </c>
       <c r="Q23">
         <v>18</v>
@@ -8251,7 +8251,7 @@
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="str">
         <f>Regions!V3</f>
-        <v>IE-WD</v>
+        <v/>
       </c>
       <c r="Q24">
         <v>19</v>
@@ -8264,7 +8264,7 @@
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="str">
         <f>Regions!W3</f>
-        <v>IE-G</v>
+        <v/>
       </c>
       <c r="Q25">
         <v>20</v>
@@ -8277,7 +8277,7 @@
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="str">
         <f>Regions!X3</f>
-        <v>IE-LM</v>
+        <v/>
       </c>
       <c r="Q26">
         <v>21</v>
@@ -8290,7 +8290,7 @@
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="str">
         <f>Regions!Y3</f>
-        <v>IE-MO</v>
+        <v/>
       </c>
       <c r="Q27">
         <v>22</v>
@@ -8303,7 +8303,7 @@
       <c r="A28" s="7"/>
       <c r="C28" s="8" t="str">
         <f>Regions!Z3</f>
-        <v>IE-RN</v>
+        <v/>
       </c>
       <c r="Q28">
         <v>23</v>
@@ -8316,28 +8316,28 @@
       <c r="A29" s="7"/>
       <c r="C29" s="8" t="str">
         <f>Regions!AA3</f>
-        <v>IE-SO</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A30" s="7"/>
       <c r="C30" s="8" t="str">
         <f>Regions!AB3</f>
-        <v>IE-CN</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A31" s="7"/>
       <c r="C31" s="8" t="str">
         <f>Regions!AC3</f>
-        <v>IE-DL</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A32" s="7"/>
       <c r="C32" s="8" t="str">
         <f>Regions!AD3</f>
-        <v>IE-MN</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
@@ -10642,4 +10642,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Change ActivePDef in SysSettings to P22
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\times-ireland-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F208A0A1-9534-4798-A8D6-053FF73568D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B7135D-CBBF-499B-B590-6F6EE3ABBDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -1569,7 +1569,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
+          <xdr:colOff>31750</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4255,21 +4255,21 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="21.73046875" style="43" customWidth="1"/>
-    <col min="5" max="6" width="14.1328125" style="43" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" style="43" customWidth="1"/>
-    <col min="8" max="10" width="8.1328125" style="43" customWidth="1"/>
-    <col min="11" max="11" width="9.73046875" style="43" customWidth="1"/>
-    <col min="12" max="12" width="8.1328125" style="43" customWidth="1"/>
+    <col min="1" max="4" width="21.7265625" style="43" customWidth="1"/>
+    <col min="5" max="6" width="14.08984375" style="43" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" style="43" customWidth="1"/>
+    <col min="8" max="10" width="8.08984375" style="43" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" style="43" customWidth="1"/>
+    <col min="12" max="12" width="8.08984375" style="43" customWidth="1"/>
     <col min="13" max="13" width="10" style="43" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" style="43" customWidth="1"/>
-    <col min="15" max="15" width="13.3984375" style="43" customWidth="1"/>
-    <col min="16" max="16384" width="8.86328125" style="43"/>
+    <col min="14" max="14" width="11.36328125" style="43" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" style="43" customWidth="1"/>
+    <col min="16" max="16384" width="8.81640625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="41"/>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -4297,7 +4297,7 @@
       <c r="Y1" s="42"/>
       <c r="Z1" s="42"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -4325,7 +4325,7 @@
       <c r="Y2" s="42"/>
       <c r="Z2" s="42"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -4353,7 +4353,7 @@
       <c r="Y3" s="42"/>
       <c r="Z3" s="42"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="41"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -4381,7 +4381,7 @@
       <c r="Y4" s="42"/>
       <c r="Z4" s="42"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="41"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -4409,7 +4409,7 @@
       <c r="Y5" s="42"/>
       <c r="Z5" s="42"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="41"/>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -4437,7 +4437,7 @@
       <c r="Y6" s="42"/>
       <c r="Z6" s="42"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="41"/>
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
@@ -4465,7 +4465,7 @@
       <c r="Y7" s="42"/>
       <c r="Z7" s="42"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="41"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
@@ -4493,7 +4493,7 @@
       <c r="Y8" s="42"/>
       <c r="Z8" s="42"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="41"/>
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
@@ -4521,7 +4521,7 @@
       <c r="Y9" s="42"/>
       <c r="Z9" s="42"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="41"/>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
@@ -4549,7 +4549,7 @@
       <c r="Y10" s="42"/>
       <c r="Z10" s="42"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="41"/>
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
@@ -4577,7 +4577,7 @@
       <c r="Y11" s="42"/>
       <c r="Z11" s="42"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="41"/>
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
@@ -4605,7 +4605,7 @@
       <c r="Y12" s="42"/>
       <c r="Z12" s="42"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="41"/>
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
@@ -4633,7 +4633,7 @@
       <c r="Y13" s="42"/>
       <c r="Z13" s="42"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="41"/>
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
@@ -4661,7 +4661,7 @@
       <c r="Y14" s="42"/>
       <c r="Z14" s="42"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="41"/>
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
@@ -4689,7 +4689,7 @@
       <c r="Y15" s="42"/>
       <c r="Z15" s="42"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="58" t="s">
         <v>155</v>
       </c>
@@ -4719,7 +4719,7 @@
       <c r="Y16" s="42"/>
       <c r="Z16" s="42"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="46"/>
       <c r="B17" s="46"/>
       <c r="C17" s="46"/>
@@ -4747,7 +4747,7 @@
       <c r="Y17" s="42"/>
       <c r="Z17" s="42"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="46"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
@@ -4775,7 +4775,7 @@
       <c r="Y18" s="42"/>
       <c r="Z18" s="42"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="49" t="s">
         <v>156</v>
       </c>
@@ -4807,7 +4807,7 @@
       <c r="Y19" s="42"/>
       <c r="Z19" s="42"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="49" t="s">
         <v>157</v>
       </c>
@@ -4839,7 +4839,7 @@
       <c r="Y20" s="42"/>
       <c r="Z20" s="42"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="49" t="s">
         <v>158</v>
       </c>
@@ -4871,7 +4871,7 @@
       <c r="Y21" s="42"/>
       <c r="Z21" s="42"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="49"/>
       <c r="B22" s="52"/>
       <c r="C22" s="52"/>
@@ -4899,7 +4899,7 @@
       <c r="Y22" s="42"/>
       <c r="Z22" s="42"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="49" t="s">
         <v>159</v>
       </c>
@@ -4931,7 +4931,7 @@
       <c r="Y23" s="42"/>
       <c r="Z23" s="42"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="49"/>
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
@@ -4959,7 +4959,7 @@
       <c r="Y24" s="42"/>
       <c r="Z24" s="42"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="49"/>
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
@@ -4987,7 +4987,7 @@
       <c r="Y25" s="42"/>
       <c r="Z25" s="42"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="49" t="s">
         <v>160</v>
       </c>
@@ -5019,7 +5019,7 @@
       <c r="Y26" s="42"/>
       <c r="Z26" s="42"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="49"/>
       <c r="B27" s="52"/>
       <c r="C27" s="52"/>
@@ -5047,7 +5047,7 @@
       <c r="Y27" s="42"/>
       <c r="Z27" s="42"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="49"/>
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
@@ -5075,7 +5075,7 @@
       <c r="Y28" s="42"/>
       <c r="Z28" s="42"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="49" t="s">
         <v>161</v>
       </c>
@@ -5107,7 +5107,7 @@
       <c r="Y29" s="42"/>
       <c r="Z29" s="42"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="49" t="s">
         <v>162</v>
       </c>
@@ -5139,7 +5139,7 @@
       <c r="Y30" s="42"/>
       <c r="Z30" s="42"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="49" t="s">
         <v>164</v>
       </c>
@@ -5171,7 +5171,7 @@
       <c r="Y31" s="42"/>
       <c r="Z31" s="42"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="55"/>
       <c r="B32" s="56" t="s">
         <v>166</v>
@@ -5201,7 +5201,7 @@
       <c r="Y32" s="42"/>
       <c r="Z32" s="42"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="41"/>
       <c r="B33" s="41"/>
       <c r="C33" s="41"/>
@@ -5229,7 +5229,7 @@
       <c r="Y33" s="42"/>
       <c r="Z33" s="42"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="41"/>
       <c r="B34" s="41"/>
       <c r="C34" s="41"/>
@@ -5257,7 +5257,7 @@
       <c r="Y34" s="42"/>
       <c r="Z34" s="42"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="41"/>
       <c r="B35" s="41"/>
       <c r="C35" s="41"/>
@@ -5285,7 +5285,7 @@
       <c r="Y35" s="42"/>
       <c r="Z35" s="42"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="41"/>
       <c r="B36" s="41"/>
       <c r="C36" s="41"/>
@@ -5313,7 +5313,7 @@
       <c r="Y36" s="42"/>
       <c r="Z36" s="42"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="41"/>
       <c r="B37" s="41"/>
       <c r="C37" s="41"/>
@@ -5341,7 +5341,7 @@
       <c r="Y37" s="42"/>
       <c r="Z37" s="42"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="41"/>
       <c r="B38" s="41"/>
       <c r="C38" s="41"/>
@@ -5369,7 +5369,7 @@
       <c r="Y38" s="42"/>
       <c r="Z38" s="42"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="41"/>
       <c r="B39" s="41"/>
       <c r="C39" s="41"/>
@@ -5397,7 +5397,7 @@
       <c r="Y39" s="42"/>
       <c r="Z39" s="42"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="41"/>
       <c r="B40" s="41"/>
       <c r="C40" s="41"/>
@@ -5425,7 +5425,7 @@
       <c r="Y40" s="42"/>
       <c r="Z40" s="42"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="41"/>
       <c r="B41" s="41"/>
       <c r="C41" s="41"/>
@@ -5453,7 +5453,7 @@
       <c r="Y41" s="42"/>
       <c r="Z41" s="42"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="41"/>
       <c r="B42" s="41"/>
       <c r="C42" s="41"/>
@@ -5481,7 +5481,7 @@
       <c r="Y42" s="42"/>
       <c r="Z42" s="42"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="42"/>
       <c r="B43" s="42"/>
       <c r="C43" s="42"/>
@@ -5509,7 +5509,7 @@
       <c r="Y43" s="42"/>
       <c r="Z43" s="42"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="42"/>
       <c r="B44" s="42"/>
       <c r="C44" s="42"/>
@@ -5537,7 +5537,7 @@
       <c r="Y44" s="42"/>
       <c r="Z44" s="42"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="42"/>
       <c r="B45" s="42"/>
       <c r="C45" s="42"/>
@@ -5565,7 +5565,7 @@
       <c r="Y45" s="42"/>
       <c r="Z45" s="42"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="42"/>
       <c r="B46" s="42"/>
       <c r="C46" s="42"/>
@@ -5593,7 +5593,7 @@
       <c r="Y46" s="42"/>
       <c r="Z46" s="42"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="42"/>
       <c r="B47" s="42"/>
       <c r="C47" s="42"/>
@@ -5621,7 +5621,7 @@
       <c r="Y47" s="42"/>
       <c r="Z47" s="42"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="42"/>
       <c r="B48" s="42"/>
       <c r="C48" s="42"/>
@@ -5649,7 +5649,7 @@
       <c r="Y48" s="42"/>
       <c r="Z48" s="42"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="42"/>
       <c r="B49" s="42"/>
       <c r="C49" s="42"/>
@@ -5677,7 +5677,7 @@
       <c r="Y49" s="42"/>
       <c r="Z49" s="42"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="42"/>
       <c r="B50" s="42"/>
       <c r="C50" s="42"/>
@@ -5705,7 +5705,7 @@
       <c r="Y50" s="42"/>
       <c r="Z50" s="42"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="42"/>
       <c r="B51" s="42"/>
       <c r="C51" s="42"/>
@@ -5733,7 +5733,7 @@
       <c r="Y51" s="42"/>
       <c r="Z51" s="42"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="42"/>
       <c r="B52" s="42"/>
       <c r="C52" s="42"/>
@@ -5761,7 +5761,7 @@
       <c r="Y52" s="42"/>
       <c r="Z52" s="42"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="42"/>
       <c r="B53" s="42"/>
       <c r="C53" s="42"/>
@@ -5789,7 +5789,7 @@
       <c r="Y53" s="42"/>
       <c r="Z53" s="42"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="42"/>
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
@@ -5817,7 +5817,7 @@
       <c r="Y54" s="42"/>
       <c r="Z54" s="42"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="42"/>
       <c r="B55" s="42"/>
       <c r="C55" s="42"/>
@@ -5845,7 +5845,7 @@
       <c r="Y55" s="42"/>
       <c r="Z55" s="42"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="42"/>
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
@@ -5873,7 +5873,7 @@
       <c r="Y56" s="42"/>
       <c r="Z56" s="42"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="42"/>
       <c r="B57" s="42"/>
       <c r="C57" s="42"/>
@@ -5901,7 +5901,7 @@
       <c r="Y57" s="42"/>
       <c r="Z57" s="42"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="42"/>
       <c r="B58" s="42"/>
       <c r="C58" s="42"/>
@@ -5929,7 +5929,7 @@
       <c r="Y58" s="42"/>
       <c r="Z58" s="42"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="42"/>
       <c r="B59" s="42"/>
       <c r="C59" s="42"/>
@@ -5957,7 +5957,7 @@
       <c r="Y59" s="42"/>
       <c r="Z59" s="42"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="42"/>
       <c r="B60" s="42"/>
       <c r="C60" s="42"/>
@@ -5985,7 +5985,7 @@
       <c r="Y60" s="42"/>
       <c r="Z60" s="42"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="42"/>
       <c r="B61" s="42"/>
       <c r="C61" s="42"/>
@@ -6013,7 +6013,7 @@
       <c r="Y61" s="42"/>
       <c r="Z61" s="42"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="42"/>
       <c r="B62" s="42"/>
       <c r="C62" s="42"/>
@@ -6041,7 +6041,7 @@
       <c r="Y62" s="42"/>
       <c r="Z62" s="42"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="42"/>
       <c r="B63" s="42"/>
       <c r="C63" s="42"/>
@@ -6069,7 +6069,7 @@
       <c r="Y63" s="42"/>
       <c r="Z63" s="42"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="42"/>
       <c r="B64" s="42"/>
       <c r="C64" s="42"/>
@@ -6097,7 +6097,7 @@
       <c r="Y64" s="42"/>
       <c r="Z64" s="42"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="42"/>
       <c r="B65" s="42"/>
       <c r="C65" s="42"/>
@@ -6125,7 +6125,7 @@
       <c r="Y65" s="42"/>
       <c r="Z65" s="42"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="42"/>
       <c r="B66" s="42"/>
       <c r="C66" s="42"/>
@@ -6153,7 +6153,7 @@
       <c r="Y66" s="42"/>
       <c r="Z66" s="42"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="42"/>
       <c r="B67" s="42"/>
       <c r="C67" s="42"/>
@@ -6181,7 +6181,7 @@
       <c r="Y67" s="42"/>
       <c r="Z67" s="42"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="42"/>
       <c r="B68" s="42"/>
       <c r="C68" s="42"/>
@@ -6209,7 +6209,7 @@
       <c r="Y68" s="42"/>
       <c r="Z68" s="42"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="42"/>
       <c r="B69" s="42"/>
       <c r="C69" s="42"/>
@@ -6237,7 +6237,7 @@
       <c r="Y69" s="42"/>
       <c r="Z69" s="42"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="42"/>
       <c r="B70" s="42"/>
       <c r="C70" s="42"/>
@@ -6265,7 +6265,7 @@
       <c r="Y70" s="42"/>
       <c r="Z70" s="42"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="42"/>
       <c r="B71" s="42"/>
       <c r="C71" s="42"/>
@@ -6293,7 +6293,7 @@
       <c r="Y71" s="42"/>
       <c r="Z71" s="42"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="42"/>
       <c r="B72" s="42"/>
       <c r="C72" s="42"/>
@@ -6321,7 +6321,7 @@
       <c r="Y72" s="42"/>
       <c r="Z72" s="42"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="42"/>
       <c r="B73" s="42"/>
       <c r="C73" s="42"/>
@@ -6349,7 +6349,7 @@
       <c r="Y73" s="42"/>
       <c r="Z73" s="42"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="42"/>
       <c r="B74" s="42"/>
       <c r="C74" s="42"/>
@@ -6377,7 +6377,7 @@
       <c r="Y74" s="42"/>
       <c r="Z74" s="42"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="42"/>
       <c r="B75" s="42"/>
       <c r="C75" s="42"/>
@@ -6405,7 +6405,7 @@
       <c r="Y75" s="42"/>
       <c r="Z75" s="42"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="42"/>
       <c r="B76" s="42"/>
       <c r="C76" s="42"/>
@@ -6433,7 +6433,7 @@
       <c r="Y76" s="42"/>
       <c r="Z76" s="42"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="42"/>
       <c r="B77" s="42"/>
       <c r="C77" s="42"/>
@@ -6461,7 +6461,7 @@
       <c r="Y77" s="42"/>
       <c r="Z77" s="42"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="42"/>
       <c r="B78" s="42"/>
       <c r="C78" s="42"/>
@@ -6489,7 +6489,7 @@
       <c r="Y78" s="42"/>
       <c r="Z78" s="42"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="42"/>
       <c r="B79" s="42"/>
       <c r="C79" s="42"/>
@@ -6517,7 +6517,7 @@
       <c r="Y79" s="42"/>
       <c r="Z79" s="42"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="42"/>
       <c r="B80" s="42"/>
       <c r="C80" s="42"/>
@@ -6545,7 +6545,7 @@
       <c r="Y80" s="42"/>
       <c r="Z80" s="42"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="42"/>
       <c r="B81" s="42"/>
       <c r="C81" s="42"/>
@@ -6573,7 +6573,7 @@
       <c r="Y81" s="42"/>
       <c r="Z81" s="42"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="42"/>
       <c r="B82" s="42"/>
       <c r="C82" s="42"/>
@@ -6601,7 +6601,7 @@
       <c r="Y82" s="42"/>
       <c r="Z82" s="42"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="42"/>
@@ -6629,7 +6629,7 @@
       <c r="Y83" s="42"/>
       <c r="Z83" s="42"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="42"/>
       <c r="B84" s="42"/>
       <c r="C84" s="42"/>
@@ -6657,7 +6657,7 @@
       <c r="Y84" s="42"/>
       <c r="Z84" s="42"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="42"/>
       <c r="B85" s="42"/>
       <c r="C85" s="42"/>
@@ -6685,7 +6685,7 @@
       <c r="Y85" s="42"/>
       <c r="Z85" s="42"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="42"/>
       <c r="B86" s="42"/>
       <c r="C86" s="42"/>
@@ -6713,7 +6713,7 @@
       <c r="Y86" s="42"/>
       <c r="Z86" s="42"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="42"/>
       <c r="B87" s="42"/>
       <c r="C87" s="42"/>
@@ -6741,7 +6741,7 @@
       <c r="Y87" s="42"/>
       <c r="Z87" s="42"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="42"/>
       <c r="B88" s="42"/>
       <c r="C88" s="42"/>
@@ -6769,7 +6769,7 @@
       <c r="Y88" s="42"/>
       <c r="Z88" s="42"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="42"/>
       <c r="B89" s="42"/>
       <c r="C89" s="42"/>
@@ -6797,7 +6797,7 @@
       <c r="Y89" s="42"/>
       <c r="Z89" s="42"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="42"/>
       <c r="B90" s="42"/>
       <c r="C90" s="42"/>
@@ -6825,7 +6825,7 @@
       <c r="Y90" s="42"/>
       <c r="Z90" s="42"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="42"/>
       <c r="B91" s="42"/>
       <c r="C91" s="42"/>
@@ -6853,7 +6853,7 @@
       <c r="Y91" s="42"/>
       <c r="Z91" s="42"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="42"/>
       <c r="B92" s="42"/>
       <c r="C92" s="42"/>
@@ -6881,7 +6881,7 @@
       <c r="Y92" s="42"/>
       <c r="Z92" s="42"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="42"/>
       <c r="B93" s="42"/>
       <c r="C93" s="42"/>
@@ -6909,7 +6909,7 @@
       <c r="Y93" s="42"/>
       <c r="Z93" s="42"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" s="42"/>
       <c r="B94" s="42"/>
       <c r="C94" s="42"/>
@@ -6937,7 +6937,7 @@
       <c r="Y94" s="42"/>
       <c r="Z94" s="42"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" s="42"/>
       <c r="B95" s="42"/>
       <c r="C95" s="42"/>
@@ -6965,7 +6965,7 @@
       <c r="Y95" s="42"/>
       <c r="Z95" s="42"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="42"/>
       <c r="B96" s="42"/>
       <c r="C96" s="42"/>
@@ -6993,7 +6993,7 @@
       <c r="Y96" s="42"/>
       <c r="Z96" s="42"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="42"/>
       <c r="B97" s="42"/>
       <c r="C97" s="42"/>
@@ -7021,7 +7021,7 @@
       <c r="Y97" s="42"/>
       <c r="Z97" s="42"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98" s="42"/>
       <c r="B98" s="42"/>
       <c r="C98" s="42"/>
@@ -7049,7 +7049,7 @@
       <c r="Y98" s="42"/>
       <c r="Z98" s="42"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99" s="42"/>
       <c r="B99" s="42"/>
       <c r="C99" s="42"/>
@@ -7102,42 +7102,42 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" customWidth="1"/>
-    <col min="2" max="2" width="11.73046875" customWidth="1"/>
-    <col min="3" max="3" width="3.1328125" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" customWidth="1"/>
-    <col min="5" max="5" width="6.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="3" max="3" width="3.08984375" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" customWidth="1"/>
+    <col min="5" max="5" width="6.36328125" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="5.73046875" customWidth="1"/>
-    <col min="8" max="8" width="5.86328125" customWidth="1"/>
-    <col min="9" max="9" width="5.3984375" customWidth="1"/>
-    <col min="10" max="11" width="5.73046875" customWidth="1"/>
-    <col min="12" max="12" width="6.59765625" customWidth="1"/>
+    <col min="7" max="7" width="5.7265625" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" customWidth="1"/>
+    <col min="9" max="9" width="5.36328125" customWidth="1"/>
+    <col min="10" max="11" width="5.7265625" customWidth="1"/>
+    <col min="12" max="12" width="6.6328125" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.73046875" customWidth="1"/>
-    <col min="15" max="15" width="6.59765625" customWidth="1"/>
-    <col min="16" max="16" width="7.1328125" customWidth="1"/>
-    <col min="17" max="17" width="5.73046875" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" customWidth="1"/>
+    <col min="15" max="15" width="6.6328125" customWidth="1"/>
+    <col min="16" max="16" width="7.08984375" customWidth="1"/>
+    <col min="17" max="17" width="5.7265625" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="5.86328125" customWidth="1"/>
-    <col min="20" max="20" width="5.59765625" customWidth="1"/>
-    <col min="21" max="21" width="5.86328125" customWidth="1"/>
-    <col min="22" max="22" width="6.73046875" customWidth="1"/>
+    <col min="19" max="19" width="5.81640625" customWidth="1"/>
+    <col min="20" max="20" width="5.6328125" customWidth="1"/>
+    <col min="21" max="21" width="5.81640625" customWidth="1"/>
+    <col min="22" max="22" width="6.7265625" customWidth="1"/>
     <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="7.59765625" customWidth="1"/>
-    <col min="25" max="25" width="6.73046875" customWidth="1"/>
+    <col min="24" max="24" width="7.6328125" customWidth="1"/>
+    <col min="25" max="25" width="6.7265625" customWidth="1"/>
     <col min="26" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.73046875" customWidth="1"/>
-    <col min="30" max="30" width="6.73046875" customWidth="1"/>
+    <col min="29" max="29" width="5.7265625" customWidth="1"/>
+    <col min="30" max="30" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="str">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -7251,13 +7251,13 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
@@ -7408,7 +7408,7 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>67</v>
       </c>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>74</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>80</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>82</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>84</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>86</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>90</v>
       </c>
@@ -7618,7 +7618,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>92</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>96</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>98</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>100</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>102</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>104</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>106</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>108</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>110</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>112</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>114</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>116</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>118</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>120</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>122</v>
       </c>
@@ -7764,7 +7764,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>31750</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -7788,16 +7788,16 @@
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" customWidth="1"/>
-    <col min="4" max="4" width="2.1328125" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="4" max="4" width="2.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
         <v>6</v>
@@ -7808,7 +7808,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="9" t="s">
         <v>12</v>
@@ -7844,7 +7844,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>37</v>
@@ -7881,7 +7881,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="str">
@@ -7910,7 +7910,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="str">
@@ -7939,7 +7939,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="str">
@@ -7968,7 +7968,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="str">
@@ -7994,7 +7994,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="str">
@@ -8020,7 +8020,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="str">
@@ -8047,7 +8047,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="str">
@@ -8068,7 +8068,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="str">
@@ -8089,7 +8089,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="str">
@@ -8110,7 +8110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="str">
@@ -8131,7 +8131,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="str">
@@ -8152,7 +8152,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="str">
@@ -8167,7 +8167,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="str">
@@ -8181,7 +8181,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="str">
@@ -8195,7 +8195,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="str">
         <f>Regions!R3</f>
@@ -8208,7 +8208,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="str">
         <f>Regions!S3</f>
@@ -8221,7 +8221,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="str">
         <f>Regions!T3</f>
@@ -8234,7 +8234,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="str">
         <f>Regions!U3</f>
@@ -8247,7 +8247,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="str">
         <f>Regions!V3</f>
@@ -8260,7 +8260,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="str">
         <f>Regions!W3</f>
@@ -8273,7 +8273,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="str">
         <f>Regions!X3</f>
@@ -8286,7 +8286,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="str">
         <f>Regions!Y3</f>
@@ -8299,7 +8299,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="C28" s="8" t="str">
         <f>Regions!Z3</f>
@@ -8312,38 +8312,38 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="C29" s="8" t="str">
         <f>Regions!AA3</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="C30" s="8" t="str">
         <f>Regions!AB3</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="C31" s="8" t="str">
         <f>Regions!AC3</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="C32" s="8" t="str">
         <f>Regions!AD3</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
@@ -8352,19 +8352,19 @@
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
     </row>
-    <row r="35" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
     </row>
   </sheetData>
@@ -8384,44 +8384,44 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:J51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="13.73046875" customWidth="1"/>
+    <col min="2" max="10" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>147</v>
       </c>
@@ -8450,7 +8450,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="13">
         <v>1</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="13">
         <v>1</v>
       </c>
@@ -8508,7 +8508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
         <v>1</v>
       </c>
@@ -8537,7 +8537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <v>20</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>20</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="13">
         <v>5</v>
       </c>
@@ -8621,7 +8621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="13">
         <v>45</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="13">
         <v>25</v>
       </c>
@@ -8673,7 +8673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="13">
         <v>5</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D22" s="13">
         <v>5</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D23" s="13">
         <v>5</v>
       </c>
@@ -8745,7 +8745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D24" s="13">
         <v>5</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E25" s="13">
         <v>5</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F26" s="13">
         <v>5</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F27" s="13">
         <v>5</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G28" s="13">
         <v>5</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G29" s="13">
         <v>5</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G30" s="13">
         <v>5</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G31" s="13">
         <v>5</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G32" s="13">
         <v>5</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" s="13">
         <v>5</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" s="13">
         <v>5</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H35" s="13">
         <v>5</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I36" s="18">
         <v>1</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I37" s="18">
         <v>1</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I38" s="18">
         <v>1</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I39" s="18">
         <v>1</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I40" s="18">
         <v>1</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I41" s="18">
         <v>1</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I42" s="18">
         <v>1</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I43" s="18">
         <v>1</v>
       </c>
@@ -8995,7 +8995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I44" s="18">
         <v>1</v>
       </c>
@@ -9003,7 +9003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
       <c r="I45" s="18">
         <v>1</v>
       </c>
@@ -9011,32 +9011,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J46" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J47" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J48" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J49" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J50" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J51" s="18">
         <v>5</v>
       </c>
@@ -9057,17 +9057,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.73046875" customWidth="1"/>
+    <col min="2" max="2" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>32</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
@@ -9131,42 +9131,42 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.1328125" customWidth="1"/>
-    <col min="6" max="6" width="10.73046875" customWidth="1"/>
-    <col min="7" max="7" width="6.3984375" customWidth="1"/>
-    <col min="8" max="8" width="6.265625" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="6.36328125" customWidth="1"/>
+    <col min="8" max="8" width="6.26953125" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
     </row>
-    <row r="4" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
     </row>
-    <row r="5" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
     </row>
-    <row r="6" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
     </row>
-    <row r="7" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
     </row>
-    <row r="8" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -9184,7 +9184,7 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
     </row>
-    <row r="9" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -9202,7 +9202,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -9220,7 +9220,7 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
     </row>
-    <row r="11" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -9238,7 +9238,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -9256,7 +9256,7 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>56</v>
       </c>
@@ -9275,7 +9275,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
     </row>
-    <row r="14" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
@@ -9295,7 +9295,7 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25" t="s">
@@ -9371,7 +9371,7 @@
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
     </row>
-    <row r="17" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25" t="s">
@@ -9397,7 +9397,7 @@
       <c r="O17" s="25"/>
       <c r="P17" s="25"/>
     </row>
-    <row r="18" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -9415,7 +9415,7 @@
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
     </row>
-    <row r="19" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -9433,7 +9433,7 @@
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
     </row>
-    <row r="20" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -9451,7 +9451,7 @@
       <c r="O20" s="25"/>
       <c r="P20" s="25"/>
     </row>
-    <row r="21" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
@@ -9469,7 +9469,7 @@
       <c r="O21" s="25"/>
       <c r="P21" s="25"/>
     </row>
-    <row r="22" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
@@ -9487,7 +9487,7 @@
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
     </row>
-    <row r="23" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -9505,7 +9505,7 @@
       <c r="O23" s="25"/>
       <c r="P23" s="25"/>
     </row>
-    <row r="24" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
@@ -9539,27 +9539,27 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.1328125" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="5" max="5" width="6.08984375" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -9579,7 +9579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="27" t="s">
@@ -9599,7 +9599,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B3,4))</f>
@@ -9617,7 +9617,7 @@
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B4,4))</f>
@@ -9635,7 +9635,7 @@
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B5,4))</f>
@@ -9653,7 +9653,7 @@
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B6,4))</f>
@@ -9671,7 +9671,7 @@
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B7,4))</f>
@@ -9689,7 +9689,7 @@
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B8,4))</f>
@@ -9707,7 +9707,7 @@
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B9,4))</f>
@@ -9725,7 +9725,7 @@
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B10,4))</f>
@@ -9743,7 +9743,7 @@
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B11,4))</f>
@@ -9761,7 +9761,7 @@
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B12,4))</f>
@@ -9779,7 +9779,7 @@
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B13,4))</f>
@@ -9797,7 +9797,7 @@
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B14,4))</f>
@@ -9815,7 +9815,7 @@
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B15,4))</f>
@@ -9833,7 +9833,7 @@
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B16,4))</f>
@@ -9851,7 +9851,7 @@
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B17,4))</f>
@@ -9869,7 +9869,7 @@
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B18,4))</f>
@@ -9887,7 +9887,7 @@
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B19,4))</f>
@@ -9905,7 +9905,7 @@
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B20,4))</f>
@@ -9923,7 +9923,7 @@
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B22,4))</f>
@@ -9941,7 +9941,7 @@
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="C26" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B23,4))</f>
         <v>MEUR2020</v>
@@ -9958,7 +9958,7 @@
         <v>0.9783730634328176</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="C27" s="7" t="str">
         <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B24,4))</f>
         <v>MEUR2021</v>
@@ -9975,16 +9975,16 @@
         <v>0.95079986728164989</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B34" s="26"/>
     </row>
   </sheetData>
@@ -10003,12 +10003,12 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.59765625" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
@@ -10019,7 +10019,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>172</v>
       </c>
@@ -10086,7 +10086,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="str">
         <f>Constants!C7</f>
         <v>MEUR2000</v>
@@ -10116,7 +10116,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="str">
         <f>Constants!C8</f>
         <v>MEUR2001</v>
@@ -10146,7 +10146,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="str">
         <f>Constants!C9</f>
         <v>MEUR2002</v>
@@ -10161,7 +10161,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="str">
         <f>Constants!C10</f>
         <v>MEUR2003</v>
@@ -10176,7 +10176,7 @@
         <v>41.87</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="str">
         <f>Constants!C11</f>
         <v>MEUR2004</v>
@@ -10191,7 +10191,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="str">
         <f>Constants!C12</f>
         <v>MEUR2005</v>
@@ -10206,7 +10206,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="str">
         <f>Constants!C13</f>
         <v>MEUR2006</v>
@@ -10221,7 +10221,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="str">
         <f>Constants!C14</f>
         <v>MEUR2007</v>
@@ -10236,7 +10236,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="str">
         <f>Constants!C15</f>
         <v>MEUR2008</v>
@@ -10251,7 +10251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="str">
         <f>Constants!C16</f>
         <v>MEUR2009</v>
@@ -10266,7 +10266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="str">
         <f>Constants!C17</f>
         <v>MEUR2010</v>
@@ -10281,61 +10281,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="str">
         <f>Constants!C18</f>
         <v>MEUR2011</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="str">
         <f>Constants!C19</f>
         <v>MEUR2012</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="str">
         <f>Constants!C20</f>
         <v>MEUR2013</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="str">
         <f>Constants!C21</f>
         <v>MEUR2014</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="str">
         <f>Constants!C22</f>
         <v>MEUR2015</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="str">
         <f>Constants!C23</f>
         <v>MEUR2016</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="str">
         <f>Constants!C24</f>
         <v>MEUR2017</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="str">
         <f>Constants!C25</f>
         <v>MEUR2019</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="str">
         <f>Constants!C26</f>
         <v>MEUR2020</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="str">
         <f>Constants!C27</f>
         <v>MEUR2021</v>
@@ -10357,13 +10357,13 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.3984375" customWidth="1"/>
-    <col min="3" max="4" width="13.86328125" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" customWidth="1"/>
+    <col min="3" max="4" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="29"/>
       <c r="C2" s="30" t="s">
         <v>38</v>
@@ -10372,7 +10372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B3" s="32">
         <v>2000</v>
       </c>
@@ -10381,7 +10381,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B4" s="32">
         <v>2001</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B5" s="32">
         <v>2002</v>
       </c>
@@ -10405,7 +10405,7 @@
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B6" s="32">
         <v>2003</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B7" s="32">
         <v>2004</v>
       </c>
@@ -10429,7 +10429,7 @@
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B8" s="32">
         <v>2005</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B9" s="32">
         <v>2006</v>
       </c>
@@ -10453,7 +10453,7 @@
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B10" s="32">
         <v>2007</v>
       </c>
@@ -10465,7 +10465,7 @@
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B11" s="32">
         <v>2008</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B12" s="32">
         <v>2009</v>
       </c>
@@ -10489,7 +10489,7 @@
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B13" s="32">
         <v>2010</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B14" s="32">
         <v>2011</v>
       </c>
@@ -10513,7 +10513,7 @@
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B15" s="32">
         <v>2012</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B16" s="32">
         <v>2013</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B17" s="32">
         <v>2014</v>
       </c>
@@ -10549,7 +10549,7 @@
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B18" s="32">
         <v>2015</v>
       </c>
@@ -10561,7 +10561,7 @@
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B19" s="37">
         <v>2016</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B20" s="37">
         <v>2017</v>
       </c>
@@ -10585,7 +10585,7 @@
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B21" s="37">
         <v>2018</v>
       </c>
@@ -10597,7 +10597,7 @@
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B22" s="37">
         <v>2019</v>
       </c>
@@ -10609,7 +10609,7 @@
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B23" s="37">
         <v>2020</v>
       </c>
@@ -10621,7 +10621,7 @@
         <v>142.34518354449207</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B24" s="37">
         <v>2021</v>
       </c>
@@ -10633,7 +10633,7 @@
         <v>146.47319386728233</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B26" s="36" t="s">
         <v>40</v>
       </c>

</xml_diff>